<commit_message>
#4 closed, added number of punches to new punch card
</commit_message>
<xml_diff>
--- a/jim_info.xlsx
+++ b/jim_info.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
   <si>
     <t>Burns</t>
   </si>
@@ -43,130 +43,160 @@
     <t>Rasor</t>
   </si>
   <si>
+    <t>Johnson Jr</t>
+  </si>
+  <si>
+    <t>Marcus</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Dandy</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>TRX 3-2-1</t>
+  </si>
+  <si>
+    <t>Mahurin</t>
+  </si>
+  <si>
+    <t>Howard</t>
+  </si>
+  <si>
+    <t>Sanders</t>
+  </si>
+  <si>
+    <t>Fred</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Cave Basics</t>
+  </si>
+  <si>
+    <t>Beth</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>3-2-1</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>Kettlebells</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate </t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Monthy</t>
+  </si>
+  <si>
+    <t>Due</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Bad</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Date Joined</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Rasor III</t>
+  </si>
+  <si>
+    <t>Risor</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Weaver</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Drop In</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Rasor Jr</t>
+  </si>
+  <si>
+    <t>Idea</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
+    <t>Hamvas</t>
+  </si>
+  <si>
+    <t>Middle</t>
+  </si>
+  <si>
+    <t>Tyler</t>
+  </si>
+  <si>
+    <t>Another</t>
+  </si>
+  <si>
+    <t>Punch Card</t>
+  </si>
+  <si>
     <t>NMI</t>
-  </si>
-  <si>
-    <t>Jonathan</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Sanders</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>TRX 3-2-1</t>
-  </si>
-  <si>
-    <t>Mahurin</t>
-  </si>
-  <si>
-    <t>Howard</t>
-  </si>
-  <si>
-    <t>Fred</t>
-  </si>
-  <si>
-    <t>Dave</t>
-  </si>
-  <si>
-    <t>Mon</t>
-  </si>
-  <si>
-    <t>Cave Basics</t>
-  </si>
-  <si>
-    <t>Beth</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>Fri</t>
-  </si>
-  <si>
-    <t>3-2-1</t>
-  </si>
-  <si>
-    <t>Last</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Johnson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rate </t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>Monthy</t>
-  </si>
-  <si>
-    <t>Due</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>Hamvas</t>
-  </si>
-  <si>
-    <t>date joined</t>
-  </si>
-  <si>
-    <t>Ryan</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Weaver</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>Rasor III</t>
-  </si>
-  <si>
-    <t>Drop In</t>
-  </si>
-  <si>
-    <t>Tue</t>
-  </si>
-  <si>
-    <t>Tyler</t>
-  </si>
-  <si>
-    <t>Middle</t>
-  </si>
-  <si>
-    <t>Daniel</t>
-  </si>
-  <si>
-    <t>Kettlebells</t>
-  </si>
-  <si>
-    <t>Punch Card</t>
-  </si>
-  <si>
-    <t>Rasor Jr</t>
   </si>
   <si>
     <t>Sat</t>
@@ -304,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="20" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -315,7 +345,6 @@
     <xf applyBorder="1" applyNumberFormat="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="7" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="8" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
@@ -625,64 +654,64 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col bestFit="true" min="1" max="1" collapsed="0" width="5.5703125" customWidth="true"/>
-    <col bestFit="true" min="3" max="3" collapsed="0" width="5.5703125" customWidth="true"/>
-    <col bestFit="true" min="2" max="2" collapsed="0" width="10.7109375" customWidth="true"/>
-    <col bestFit="true" min="5" max="5" collapsed="0" width="5.5703125" customWidth="true"/>
-    <col bestFit="true" min="4" max="4" collapsed="0" width="10.7109375" customWidth="true"/>
-    <col bestFit="true" min="7" max="7" collapsed="0" width="5.85546875" customWidth="true"/>
-    <col max="6" collapsed="5" customWidth="true" width="9.140625" min="6"/>
-    <col bestFit="true" min="9" max="9" collapsed="0" width="5.5703125" customWidth="true"/>
+    <col max="1" collapsed="0" customWidth="true" width="5.5703125" min="1"/>
+    <col max="3" collapsed="0" customWidth="true" width="5.5703125" min="3"/>
+    <col max="2" collapsed="0" customWidth="true" width="10.7109375" min="2"/>
+    <col max="5" collapsed="0" customWidth="true" width="5.5703125" min="5"/>
+    <col max="4" collapsed="0" customWidth="true" width="10.7109375" min="4"/>
+    <col max="7" collapsed="0" customWidth="true" width="5.85546875" min="7"/>
+    <col max="6" collapsed="0" customWidth="true" width="9.140625" min="6"/>
+    <col max="9" collapsed="0" customWidth="true" width="5.5703125" min="9"/>
     <col max="8" collapsed="0" customWidth="true" width="9.140625" min="8"/>
-    <col bestFit="true" min="11" max="11" collapsed="0" width="5.5703125" customWidth="true"/>
-    <col bestFit="true" min="10" max="10" collapsed="0" width="10.7109375" customWidth="true"/>
-    <col bestFit="true" min="13" max="13" collapsed="0" width="4.28515625" customWidth="true"/>
-    <col bestFit="true" min="12" max="12" collapsed="0" width="11.0" customWidth="true"/>
-    <col bestFit="true" min="14" max="14" collapsed="0" width="5.0" customWidth="true"/>
+    <col max="11" collapsed="0" customWidth="true" width="5.5703125" min="11"/>
+    <col max="10" collapsed="0" customWidth="true" width="10.7109375" min="10"/>
+    <col max="13" collapsed="0" customWidth="true" width="4.28515625" min="13"/>
+    <col max="12" collapsed="0" customWidth="true" width="11.0" min="12"/>
+    <col max="14" collapsed="0" customWidth="true" width="5.0" min="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c s="9" r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c s="11" r="B1" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c s="10" r="B1" t="s">
+        <v>25</v>
       </c>
       <c s="9" r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c s="11" r="D1" t="s">
-        <v>21</v>
+        <v>53</v>
+      </c>
+      <c s="10" r="D1" t="s">
+        <v>25</v>
       </c>
       <c s="9" r="E1" t="s">
         <v>1</v>
       </c>
-      <c s="11" r="F1" t="s">
-        <v>21</v>
+      <c s="10" r="F1" t="s">
+        <v>25</v>
       </c>
       <c s="9" r="G1" t="s">
         <v>6</v>
       </c>
-      <c s="11" r="H1" t="s">
-        <v>21</v>
+      <c s="10" r="H1" t="s">
+        <v>25</v>
       </c>
       <c s="9" r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c s="11" r="J1" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c s="10" r="J1" t="s">
+        <v>25</v>
       </c>
       <c s="9" r="K1" t="s">
-        <v>50</v>
-      </c>
-      <c s="11" r="L1" t="s">
-        <v>21</v>
+        <v>60</v>
+      </c>
+      <c s="10" r="L1" t="s">
+        <v>25</v>
       </c>
       <c s="9" r="M1" t="s">
         <v>3</v>
       </c>
-      <c s="11" r="N1" t="s">
-        <v>21</v>
+      <c s="10" r="N1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -696,7 +725,7 @@
         <v>0.375</v>
       </c>
       <c s="4" r="D2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c s="1" r="E2" t="n">
         <v>0.4166666666666667</v>
@@ -714,7 +743,7 @@
         <v>0.375</v>
       </c>
       <c s="4" r="J2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c s="1" r="K2" t="n">
         <v>0.4166666666666667</v>
@@ -730,7 +759,7 @@
         <v>0.7291666666666666</v>
       </c>
       <c s="4" r="B3" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c s="1" r="C3" t="n">
         <v>0.7291666666666666</v>
@@ -742,7 +771,7 @@
         <v>0.7708333333333334</v>
       </c>
       <c s="4" r="F3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c s="1" r="G3" t="n">
         <v>0.7708333333333334</v>
@@ -754,13 +783,13 @@
         <v>0.4166666666666667</v>
       </c>
       <c s="4" r="J3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c s="1" r="K3" t="n">
         <v>0.4583333333333333</v>
       </c>
       <c s="4" r="L3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c s="1" r="M3" t="s"/>
       <c s="4" r="N3" t="s"/>
@@ -820,13 +849,13 @@
     <row r="7" spans="1:14">
       <c s="1" r="A7" t="s"/>
       <c s="4" r="B7" t="s"/>
-      <c s="12" r="C7" t="s"/>
+      <c s="11" r="C7" t="s"/>
       <c s="4" r="D7" t="s"/>
       <c s="1" r="E7" t="s"/>
       <c s="4" r="F7" t="s"/>
       <c s="1" r="G7" t="s"/>
       <c s="4" r="H7" t="s"/>
-      <c s="12" r="I7" t="s"/>
+      <c s="11" r="I7" t="s"/>
       <c s="4" r="J7" t="s"/>
       <c s="1" r="K7" t="s"/>
       <c s="4" r="L7" t="s"/>
@@ -834,99 +863,99 @@
       <c s="4" r="N7" t="s"/>
     </row>
     <row r="8" spans="1:14">
-      <c s="12" r="A8" t="s"/>
+      <c s="11" r="A8" t="s"/>
       <c s="4" r="B8" t="s"/>
-      <c s="12" r="C8" t="s"/>
+      <c s="11" r="C8" t="s"/>
       <c s="4" r="D8" t="s"/>
       <c s="1" r="E8" t="s"/>
       <c s="4" r="F8" t="s"/>
-      <c s="12" r="G8" t="s"/>
+      <c s="11" r="G8" t="s"/>
       <c s="4" r="H8" t="s"/>
-      <c s="12" r="I8" t="s"/>
+      <c s="11" r="I8" t="s"/>
       <c s="4" r="J8" t="s"/>
-      <c s="12" r="K8" t="s"/>
+      <c s="11" r="K8" t="s"/>
       <c s="4" r="L8" t="s"/>
-      <c s="12" r="M8" t="s"/>
+      <c s="11" r="M8" t="s"/>
       <c s="4" r="N8" t="s"/>
     </row>
     <row r="9" spans="1:14">
-      <c s="12" r="A9" t="s"/>
+      <c s="11" r="A9" t="s"/>
       <c s="4" r="B9" t="s"/>
-      <c s="12" r="C9" t="s"/>
+      <c s="11" r="C9" t="s"/>
       <c s="4" r="D9" t="s"/>
-      <c s="12" r="E9" t="s"/>
+      <c s="11" r="E9" t="s"/>
       <c s="4" r="F9" t="s"/>
-      <c s="12" r="G9" t="s"/>
+      <c s="11" r="G9" t="s"/>
       <c s="4" r="H9" t="s"/>
-      <c s="12" r="I9" t="s"/>
+      <c s="11" r="I9" t="s"/>
       <c s="4" r="J9" t="s"/>
-      <c s="12" r="K9" t="s"/>
+      <c s="11" r="K9" t="s"/>
       <c s="4" r="L9" t="s"/>
-      <c s="12" r="M9" t="s"/>
+      <c s="11" r="M9" t="s"/>
       <c s="4" r="N9" t="s"/>
     </row>
     <row r="10" spans="1:14">
-      <c s="12" r="A10" t="s"/>
+      <c s="11" r="A10" t="s"/>
       <c s="4" r="B10" t="s"/>
-      <c s="12" r="C10" t="s"/>
+      <c s="11" r="C10" t="s"/>
       <c s="4" r="D10" t="s"/>
-      <c s="12" r="E10" t="s"/>
+      <c s="11" r="E10" t="s"/>
       <c s="4" r="F10" t="s"/>
-      <c s="12" r="G10" t="s"/>
+      <c s="11" r="G10" t="s"/>
       <c s="4" r="H10" t="s"/>
-      <c s="12" r="I10" t="s"/>
+      <c s="11" r="I10" t="s"/>
       <c s="4" r="J10" t="s"/>
-      <c s="12" r="K10" t="s"/>
+      <c s="11" r="K10" t="s"/>
       <c s="4" r="L10" t="s"/>
-      <c s="12" r="M10" t="s"/>
+      <c s="11" r="M10" t="s"/>
       <c s="4" r="N10" t="s"/>
     </row>
     <row r="11" spans="1:14">
-      <c s="12" r="A11" t="s"/>
+      <c s="11" r="A11" t="s"/>
       <c s="4" r="B11" t="s"/>
-      <c s="12" r="C11" t="s"/>
+      <c s="11" r="C11" t="s"/>
       <c s="4" r="D11" t="s"/>
-      <c s="12" r="E11" t="s"/>
+      <c s="11" r="E11" t="s"/>
       <c s="4" r="F11" t="s"/>
-      <c s="12" r="G11" t="s"/>
+      <c s="11" r="G11" t="s"/>
       <c s="4" r="H11" t="s"/>
-      <c s="12" r="I11" t="s"/>
+      <c s="11" r="I11" t="s"/>
       <c s="4" r="J11" t="s"/>
-      <c s="12" r="K11" t="s"/>
+      <c s="11" r="K11" t="s"/>
       <c s="4" r="L11" t="s"/>
-      <c s="12" r="M11" t="s"/>
+      <c s="11" r="M11" t="s"/>
       <c s="4" r="N11" t="s"/>
     </row>
     <row r="12" spans="1:14">
-      <c s="12" r="A12" t="s"/>
+      <c s="11" r="A12" t="s"/>
       <c s="4" r="B12" t="s"/>
-      <c s="12" r="C12" t="s"/>
+      <c s="11" r="C12" t="s"/>
       <c s="4" r="D12" t="s"/>
-      <c s="12" r="E12" t="s"/>
+      <c s="11" r="E12" t="s"/>
       <c s="4" r="F12" t="s"/>
-      <c s="12" r="G12" t="s"/>
+      <c s="11" r="G12" t="s"/>
       <c s="4" r="H12" t="s"/>
-      <c s="12" r="I12" t="s"/>
+      <c s="11" r="I12" t="s"/>
       <c s="4" r="J12" t="s"/>
-      <c s="12" r="K12" t="s"/>
+      <c s="11" r="K12" t="s"/>
       <c s="4" r="L12" t="s"/>
-      <c s="12" r="M12" t="s"/>
+      <c s="11" r="M12" t="s"/>
       <c s="4" r="N12" t="s"/>
     </row>
     <row r="13" spans="1:14">
-      <c s="12" r="A13" t="s"/>
+      <c s="11" r="A13" t="s"/>
       <c s="4" r="B13" t="s"/>
-      <c s="12" r="C13" t="s"/>
+      <c s="11" r="C13" t="s"/>
       <c s="4" r="D13" t="s"/>
-      <c s="12" r="E13" t="s"/>
+      <c s="11" r="E13" t="s"/>
       <c s="4" r="F13" t="s"/>
-      <c s="12" r="G13" t="s"/>
+      <c s="11" r="G13" t="s"/>
       <c s="4" r="H13" t="s"/>
-      <c s="12" r="I13" t="s"/>
+      <c s="11" r="I13" t="s"/>
       <c s="4" r="J13" t="s"/>
-      <c s="12" r="K13" t="s"/>
+      <c s="11" r="K13" t="s"/>
       <c s="4" r="L13" t="s"/>
-      <c s="12" r="M13" t="s"/>
+      <c s="11" r="M13" t="s"/>
       <c s="4" r="N13" t="s"/>
     </row>
     <row r="14" spans="1:14">
@@ -970,18 +999,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c s="9" r="A1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c s="3" r="B1" t="s">
-        <v>27</v>
-      </c>
-      <c s="11" r="C1" t="s">
         <v>32</v>
+      </c>
+      <c s="10" r="C1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B2" t="n">
         <v>85</v>
@@ -992,7 +1021,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B3" t="n">
         <v>100</v>
@@ -1000,7 +1029,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B4" t="n">
         <v>12</v>
@@ -1016,7 +1045,7 @@
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1" activeCell="A1"/>
@@ -1024,7 +1053,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="1" collapsed="0" customWidth="true" width="10.28515625" min="1"/>
+    <col max="1" collapsed="0" customWidth="true" width="10.140625" min="1"/>
     <col max="3" collapsed="0" customWidth="true" width="7.28515625" min="3"/>
     <col max="2" collapsed="0" customWidth="true" width="10.42578125" min="2"/>
     <col max="5" collapsed="0" customWidth="true" width="20.28515625" min="5"/>
@@ -1034,86 +1063,86 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c s="6" r="A1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c s="6" r="B1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c s="6" r="C1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c s="6" r="D1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c s="6" r="E1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c s="10" r="E2" t="n">
-        <v>41455</v>
+        <v>49</v>
+      </c>
+      <c s="8" r="E2" t="n">
+        <v>41496.0</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c s="5" r="C3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c s="10" r="E3" t="n">
+      <c s="8" r="E3" t="n">
         <v>41435</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c s="10" r="E4" t="n">
+      <c s="8" r="E4" t="n">
         <v>41450</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
       <c r="D5" t="s">
-        <v>48</v>
-      </c>
-      <c s="10" r="E5" t="n">
+        <v>58</v>
+      </c>
+      <c s="8" r="E5" t="n">
         <v>41429</v>
       </c>
     </row>
@@ -1122,15 +1151,15 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c s="10" r="C6" t="s">
-        <v>37</v>
+        <v>47</v>
+      </c>
+      <c s="8" r="C6" t="s">
+        <v>45</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c s="10" r="E6" t="n">
+      <c s="8" r="E6" t="n">
         <v>41450</v>
       </c>
     </row>
@@ -1139,32 +1168,32 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c s="10" r="E7" t="n">
+      <c s="8" r="E7" t="n">
         <v>41450</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
-      </c>
-      <c s="10" r="E8" t="n">
+        <v>49</v>
+      </c>
+      <c s="8" r="E8" t="n">
         <v>41455</v>
       </c>
     </row>
@@ -1173,84 +1202,203 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
-      </c>
-      <c s="10" r="E9" t="n">
+        <v>49</v>
+      </c>
+      <c s="8" r="E9" t="n">
         <v>41456</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
         <v>49</v>
       </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>42</v>
-      </c>
-      <c s="10" r="E10" t="n">
+      <c s="8" r="E10" t="n">
         <v>41456</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
-      </c>
-      <c s="10" r="E11" t="n">
+        <v>49</v>
+      </c>
+      <c s="8" r="E11" t="n">
         <v>41456</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
-      </c>
-      <c s="10" r="E12" t="n">
+        <v>49</v>
+      </c>
+      <c s="8" r="E12" t="n">
         <v>41464</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c s="8" r="E13" t="n">
-        <v>41476.0</v>
+        <v>41476</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c s="8" r="E14" t="n">
+        <v>41490</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c s="8" r="E15" t="n">
+        <v>41496.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c s="8" r="E16" t="n">
+        <v>41496.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c s="8" r="E17" t="n">
+        <v>41496.0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c s="8" r="E18" t="n">
+        <v>41496.0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c s="8" r="E19" t="n">
+        <v>41496.0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c s="8" r="E20" t="n">
+        <v>41496.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>